<commit_message>
Branch 13 final after updating Release
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Modal Doc.xlsx
+++ b/BballMVC/_Documentation/Modal Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D9FAE5-D6A6-45E2-BDB9-5E1E3A581384}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD101D3A-C4F1-4385-965F-8EFB903FDA9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="555" windowWidth="21600" windowHeight="15000" activeTab="3" xr2:uid="{916B6D86-6B13-4750-B471-CBED30586774}"/>
+    <workbookView xWindow="2610" yWindow="375" windowWidth="25515" windowHeight="15000" activeTab="2" xr2:uid="{916B6D86-6B13-4750-B471-CBED30586774}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Compare Rows" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="194">
   <si>
     <t>_AdjustmentsModel.html</t>
   </si>
@@ -384,9 +383,6 @@
     <t>Folder</t>
   </si>
   <si>
-    <t xml:space="preserve"> file:///D:/My%20Documents/wwwroot/Test/TtiPoc/TtiPoc/bin/Release/Publish</t>
-  </si>
-  <si>
     <t>Copied Publish to ttipoc.com in Arvixe</t>
   </si>
   <si>
@@ -748,6 +744,27 @@
   </si>
   <si>
     <t>Both</t>
+  </si>
+  <si>
+    <t>/wwwroot/Test/TtiPoc/TtiPoc/bin/Release/Publish</t>
+  </si>
+  <si>
+    <t>Click Configure to change Target location</t>
+  </si>
+  <si>
+    <t>Click Publish</t>
+  </si>
+  <si>
+    <t>T:\BballMVC</t>
+  </si>
+  <si>
+    <t>Publish to BballMVCproject</t>
+  </si>
+  <si>
+    <t>Rename BballMVCproject_yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>Try Web Deploy for TtiPoc</t>
   </si>
 </sst>
 </file>
@@ -912,6 +929,143 @@
         <a:xfrm>
           <a:off x="1219200" y="2667000"/>
           <a:ext cx="1829055" cy="1876687"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>181423</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31070519-7489-4D4C-8C5D-03210E1328A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5638800" y="2857500"/>
+          <a:ext cx="5495925" cy="3038923"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>153296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5B3171E-B6EE-4233-96A3-9283B70B940E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5638800" y="6096000"/>
+          <a:ext cx="3762375" cy="1677296"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177105</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D768A354-DADE-4498-A43F-E8562FBB5497}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9401175" y="6067425"/>
+          <a:ext cx="4086225" cy="1729680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1587,46 +1741,104 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584CC6C7-F35F-46FC-AB99-86E54A16A2C9}">
-  <dimension ref="B2:B9"/>
+  <dimension ref="B2:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="75.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="str">
+        <f>"&lt;li&gt;" &amp; B2 &amp; "&lt;/li&gt;"</f>
+        <v>&lt;li&gt;rt clk Startup proj&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C9" si="0">"&lt;li&gt;" &amp; B3 &amp; "&lt;/li&gt;"</f>
+        <v>&lt;li&gt;Publish&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Start&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Folder&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;/wwwroot/Test/TtiPoc/TtiPoc/bin/Release/Publish&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>67</v>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Copied Publish to ttipoc.com in Arvixe&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1634,7 +1846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5349101D-2782-49C6-91FF-41BEF8C11B61}">
   <dimension ref="A1:DO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -1646,348 +1858,348 @@
   <sheetData>
     <row r="1" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="L1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" t="s">
+        <v>166</v>
+      </c>
+      <c r="O1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" t="s">
+        <v>172</v>
+      </c>
+      <c r="U1" t="s">
+        <v>173</v>
+      </c>
+      <c r="V1" t="s">
+        <v>174</v>
+      </c>
+      <c r="W1" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="L1" t="s">
-        <v>165</v>
-      </c>
-      <c r="M1" t="s">
-        <v>166</v>
-      </c>
-      <c r="N1" t="s">
-        <v>167</v>
-      </c>
-      <c r="O1" t="s">
-        <v>168</v>
-      </c>
-      <c r="P1" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="R1" t="s">
-        <v>171</v>
-      </c>
-      <c r="S1" t="s">
-        <v>172</v>
-      </c>
-      <c r="T1" t="s">
-        <v>173</v>
-      </c>
-      <c r="U1" t="s">
-        <v>174</v>
-      </c>
-      <c r="V1" t="s">
-        <v>175</v>
-      </c>
-      <c r="W1" t="s">
-        <v>176</v>
-      </c>
-      <c r="X1" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>178</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>181</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>114</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>115</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>120</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>126</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>130</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>131</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>133</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>134</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>135</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>138</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>139</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>140</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>141</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>142</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>143</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>144</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>145</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>146</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>147</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>148</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>150</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DF1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="DG1" t="s">
         <v>156</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>117</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>120</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>124</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>125</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>126</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>127</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>128</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>129</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>131</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>132</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>133</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>134</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>135</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>138</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>139</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>140</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>141</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>142</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>143</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>144</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>145</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>146</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>147</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>148</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>149</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>150</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>151</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>152</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>153</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>154</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>155</v>
-      </c>
-      <c r="DF1" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
       </c>
       <c r="D2" s="5">
         <v>44248</v>
@@ -1996,10 +2208,10 @@
         <v>535</v>
       </c>
       <c r="F2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" t="s">
         <v>186</v>
-      </c>
-      <c r="G2" t="s">
-        <v>187</v>
       </c>
       <c r="H2">
         <v>3</v>
@@ -2104,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="AP2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AQ2">
         <v>114.188031098511</v>
@@ -2125,19 +2337,19 @@
         <v>233</v>
       </c>
       <c r="AW2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AX2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AY2">
         <v>4.6694591533374101</v>
       </c>
       <c r="AZ2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BA2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BB2">
         <v>0.5</v>
@@ -2302,27 +2514,27 @@
         <v>40.376964853746401</v>
       </c>
       <c r="DD2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="DE2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="DF2" s="8">
         <v>44248.667196215276</v>
       </c>
       <c r="DG2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
       </c>
       <c r="D3" s="5">
         <v>44248</v>
@@ -2331,10 +2543,10 @@
         <v>535</v>
       </c>
       <c r="F3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3" t="s">
         <v>186</v>
-      </c>
-      <c r="G3" t="s">
-        <v>187</v>
       </c>
       <c r="H3">
         <v>3</v>
@@ -2439,7 +2651,7 @@
         <v>0</v>
       </c>
       <c r="AP3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AQ3">
         <v>117.79667505539101</v>
@@ -2460,19 +2672,19 @@
         <v>233</v>
       </c>
       <c r="AW3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AX3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AY3">
         <v>6.8116055106043003</v>
       </c>
       <c r="AZ3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BA3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BB3">
         <v>0.5</v>
@@ -2637,21 +2849,21 @@
         <v>37.022812212670999</v>
       </c>
       <c r="DD3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="DE3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="DF3" s="8">
         <v>44248.642897337966</v>
       </c>
       <c r="DG3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:119" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="11" t="str">
         <f>IF(C2&lt;&gt;C3,"Diff","")</f>

</xml_diff>

<commit_message>
Rebuilt TodaysMatchups & UserLeagueParms via EF
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Modal Doc.xlsx
+++ b/BballMVC/_Documentation/Modal Doc.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D0F3D7-6994-4046-9A96-07EB8B121BB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F131D3D3-BC34-415D-A8A1-C7ED0CD186BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="1695" windowWidth="23295" windowHeight="11835" activeTab="5" xr2:uid="{916B6D86-6B13-4750-B471-CBED30586774}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" activeTab="7" xr2:uid="{916B6D86-6B13-4750-B471-CBED30586774}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Modal 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Modal 2" sheetId="2" r:id="rId2"/>
     <sheet name="Publish" sheetId="3" r:id="rId3"/>
     <sheet name="TS Doc" sheetId="6" r:id="rId4"/>
     <sheet name="Compare Rows" sheetId="5" r:id="rId5"/>
     <sheet name="DailySummary" sheetId="7" r:id="rId6"/>
+    <sheet name="xlsB" sheetId="8" r:id="rId7"/>
+    <sheet name="Pace" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="div">Pace!$M$1</definedName>
     <definedName name="header">DailySummary!$K$1:$AS$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="180">
   <si>
     <t>_AdjustmentsModel.html</t>
   </si>
@@ -746,6 +749,45 @@
 Games
 Back</t>
   </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>DIFF %</t>
+  </si>
+  <si>
+    <t>Get Last 7</t>
+  </si>
+  <si>
+    <t>Replace Klunkers w n-1</t>
+  </si>
+  <si>
+    <t>If Klunkers &gt; 1 EXIT</t>
+  </si>
+  <si>
+    <t>Col Value ==&gt;</t>
+  </si>
+  <si>
+    <t>Sum Value Diffs * Col Values</t>
+  </si>
+  <si>
+    <t>adjed</t>
+  </si>
+  <si>
+    <t>Avg Dev</t>
+  </si>
+  <si>
+    <t>From T-Sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -754,7 +796,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,8 +864,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,8 +898,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -872,11 +928,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -923,6 +990,33 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1164,6 +1258,55 @@
         <a:xfrm>
           <a:off x="3255817" y="1151659"/>
           <a:ext cx="7471325" cy="2685991"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>258147</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171660</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69524CB5-E6E7-4FFA-9BD8-1DBC1645B5A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6963747" cy="1505160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2833,7 +2976,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AT31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1:AS1"/>
     </sheetView>
   </sheetViews>
@@ -7187,4 +7330,972 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910DA3AF-4FAC-40F6-A674-BA5FA84A8F8A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F75EF2B-1769-4EC6-8EE7-0A55703BF711}">
+  <dimension ref="A1:U27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="27">
+        <v>5</v>
+      </c>
+      <c r="E1" s="27">
+        <v>6</v>
+      </c>
+      <c r="F1" s="27">
+        <v>7</v>
+      </c>
+      <c r="G1" s="27">
+        <v>8</v>
+      </c>
+      <c r="H1" s="27">
+        <v>9</v>
+      </c>
+      <c r="I1" s="27">
+        <v>10</v>
+      </c>
+      <c r="J1" s="27">
+        <v>11</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="M1" s="29">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
+        <v>170</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="P1">
+        <v>2</v>
+      </c>
+      <c r="Q1">
+        <v>3</v>
+      </c>
+      <c r="R1">
+        <v>4</v>
+      </c>
+      <c r="S1">
+        <v>5</v>
+      </c>
+      <c r="T1">
+        <v>6</v>
+      </c>
+      <c r="U1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" s="23">
+        <f>AVERAGE(D2:J2)</f>
+        <v>173.85714285714286</v>
+      </c>
+      <c r="C2" s="23">
+        <f>AVEDEV(D2:J2)</f>
+        <v>4.1632653061224483</v>
+      </c>
+      <c r="D2" s="24">
+        <v>170</v>
+      </c>
+      <c r="E2" s="24">
+        <v>165</v>
+      </c>
+      <c r="F2" s="24">
+        <v>175</v>
+      </c>
+      <c r="G2" s="24">
+        <v>180</v>
+      </c>
+      <c r="H2" s="34">
+        <v>180</v>
+      </c>
+      <c r="I2" s="24">
+        <v>175</v>
+      </c>
+      <c r="J2" s="24">
+        <v>172</v>
+      </c>
+      <c r="K2" s="25"/>
+      <c r="L2" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="M2" s="25"/>
+      <c r="N2" s="28">
+        <f>ABS(1 - (O2/L2))</f>
+        <v>1.2</v>
+      </c>
+      <c r="O2" s="31">
+        <f>SUM(P2:U2) / div</f>
+        <v>-0.1</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:P4" si="0">(E2-D2) * D$1</f>
+        <v>-25</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q4" si="1">(F2-E2) * E$1</f>
+        <v>60</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2:R4" si="2">(G2-F2) * F$1</f>
+        <v>35</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ref="S2:S9" si="3">(H2-G2) * G$1</f>
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ref="T2:T9" si="4">(I2-H2) * H$1</f>
+        <v>-45</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ref="U2:U9" si="5">(J2-I2) * I$1</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="23">
+        <f t="shared" ref="B3:B11" si="6">AVERAGE(D3:J3)</f>
+        <v>172</v>
+      </c>
+      <c r="C3" s="23">
+        <f t="shared" ref="C3:C11" si="7">AVEDEV(D3:J3)</f>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="D3" s="24">
+        <v>175</v>
+      </c>
+      <c r="E3" s="24">
+        <v>174</v>
+      </c>
+      <c r="F3" s="24">
+        <v>172</v>
+      </c>
+      <c r="G3" s="24">
+        <v>170</v>
+      </c>
+      <c r="H3" s="24">
+        <v>175</v>
+      </c>
+      <c r="I3" s="24">
+        <v>168</v>
+      </c>
+      <c r="J3" s="24">
+        <v>170</v>
+      </c>
+      <c r="K3" s="25"/>
+      <c r="L3" s="33">
+        <v>-0.5</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="28">
+        <f t="shared" ref="N3:N9" si="8">ABS(1 - (O3/L3))</f>
+        <v>0.3600000000000001</v>
+      </c>
+      <c r="O3" s="31">
+        <f>SUM(P3:U3) / div</f>
+        <v>-0.68</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="4"/>
+        <v>-63</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="23">
+        <f t="shared" si="6"/>
+        <v>176.85714285714286</v>
+      </c>
+      <c r="C4" s="23">
+        <f t="shared" si="7"/>
+        <v>3.3061224489795911</v>
+      </c>
+      <c r="D4" s="24">
+        <v>170</v>
+      </c>
+      <c r="E4" s="24">
+        <v>173</v>
+      </c>
+      <c r="F4" s="24">
+        <v>176</v>
+      </c>
+      <c r="G4" s="24">
+        <v>180</v>
+      </c>
+      <c r="H4" s="24">
+        <v>177</v>
+      </c>
+      <c r="I4" s="24">
+        <v>180</v>
+      </c>
+      <c r="J4" s="24">
+        <v>182</v>
+      </c>
+      <c r="K4" s="25"/>
+      <c r="L4" s="33">
+        <v>2</v>
+      </c>
+      <c r="M4" s="25"/>
+      <c r="N4" s="28">
+        <f t="shared" si="8"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="O4" s="31">
+        <f>SUM(P4:U4) / div</f>
+        <v>1.68</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="3"/>
+        <v>-24</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="23">
+        <f t="shared" si="6"/>
+        <v>173.14285714285714</v>
+      </c>
+      <c r="C5" s="23">
+        <f t="shared" si="7"/>
+        <v>2.6938775510204089</v>
+      </c>
+      <c r="D5" s="24">
+        <v>177</v>
+      </c>
+      <c r="E5" s="24">
+        <v>176</v>
+      </c>
+      <c r="F5" s="24">
+        <v>174</v>
+      </c>
+      <c r="G5" s="24">
+        <v>172</v>
+      </c>
+      <c r="H5" s="24">
+        <v>170</v>
+      </c>
+      <c r="I5" s="24">
+        <v>175</v>
+      </c>
+      <c r="J5" s="24">
+        <v>168</v>
+      </c>
+      <c r="K5" s="25"/>
+      <c r="L5" s="33">
+        <v>-1</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="28">
+        <f t="shared" si="8"/>
+        <v>0.43999999999999995</v>
+      </c>
+      <c r="O5" s="31">
+        <f>SUM(P5:U5) / div</f>
+        <v>-1.44</v>
+      </c>
+      <c r="P5">
+        <f>(E5-D5) * D$1</f>
+        <v>-5</v>
+      </c>
+      <c r="Q5">
+        <f>(F5-E5) * E$1</f>
+        <v>-12</v>
+      </c>
+      <c r="R5">
+        <f>(G5-F5) * F$1</f>
+        <v>-14</v>
+      </c>
+      <c r="S5">
+        <f>(H5-G5) * G$1</f>
+        <v>-16</v>
+      </c>
+      <c r="T5">
+        <f>(I5-H5) * H$1</f>
+        <v>45</v>
+      </c>
+      <c r="U5">
+        <f>(J5-I5) * I$1</f>
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="23">
+        <f t="shared" si="6"/>
+        <v>174.57142857142858</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" si="7"/>
+        <v>8.0816326530612255</v>
+      </c>
+      <c r="D6" s="24">
+        <v>165</v>
+      </c>
+      <c r="E6" s="24">
+        <v>170</v>
+      </c>
+      <c r="F6" s="24">
+        <v>173</v>
+      </c>
+      <c r="G6" s="34">
+        <v>162</v>
+      </c>
+      <c r="H6" s="24">
+        <v>180</v>
+      </c>
+      <c r="I6" s="24">
+        <v>184</v>
+      </c>
+      <c r="J6" s="24">
+        <v>188</v>
+      </c>
+      <c r="K6" s="25"/>
+      <c r="L6" s="33">
+        <v>3</v>
+      </c>
+      <c r="M6" s="25"/>
+      <c r="N6" s="28">
+        <f t="shared" ref="N6" si="9">ABS(1 - (O6/L6))</f>
+        <v>0.24</v>
+      </c>
+      <c r="O6" s="31">
+        <f>SUM(P6:U6) / div</f>
+        <v>3.72</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6" si="10">(E6-D6) * D$1</f>
+        <v>25</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6" si="11">(F6-E6) * E$1</f>
+        <v>18</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6" si="12">(G6-F6) * F$1</f>
+        <v>-77</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6" si="13">(H6-G6) * G$1</f>
+        <v>144</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6" si="14">(I6-H6) * H$1</f>
+        <v>36</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ref="U6" si="15">(J6-I6) * I$1</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="23">
+        <f t="shared" si="6"/>
+        <v>176.14285714285714</v>
+      </c>
+      <c r="C7" s="23">
+        <f t="shared" si="7"/>
+        <v>6.7346938775510194</v>
+      </c>
+      <c r="D7" s="24">
+        <v>165</v>
+      </c>
+      <c r="E7" s="24">
+        <v>170</v>
+      </c>
+      <c r="F7" s="24">
+        <v>173</v>
+      </c>
+      <c r="G7" s="34">
+        <v>173</v>
+      </c>
+      <c r="H7" s="24">
+        <v>180</v>
+      </c>
+      <c r="I7" s="24">
+        <v>184</v>
+      </c>
+      <c r="J7" s="24">
+        <v>188</v>
+      </c>
+      <c r="K7" s="25"/>
+      <c r="L7" s="33">
+        <v>3</v>
+      </c>
+      <c r="M7" s="25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N7" s="28">
+        <f t="shared" ref="N7" si="16">ABS(1 - (O7/L7))</f>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="O7" s="31">
+        <f>SUM(P7:U7) / div</f>
+        <v>3.5</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7" si="17">(E7-D7) * D$1</f>
+        <v>25</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7" si="18">(F7-E7) * E$1</f>
+        <v>18</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7" si="19">(G7-F7) * F$1</f>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7" si="20">(H7-G7) * G$1</f>
+        <v>56</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7" si="21">(I7-H7) * H$1</f>
+        <v>36</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7" si="22">(J7-I7) * I$1</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="23">
+        <f t="shared" si="6"/>
+        <v>174</v>
+      </c>
+      <c r="C8" s="23">
+        <f t="shared" si="7"/>
+        <v>4.5714285714285712</v>
+      </c>
+      <c r="D8" s="24">
+        <v>183</v>
+      </c>
+      <c r="E8" s="24">
+        <v>177</v>
+      </c>
+      <c r="F8" s="24">
+        <v>178</v>
+      </c>
+      <c r="G8" s="24">
+        <v>173</v>
+      </c>
+      <c r="H8" s="24">
+        <v>168</v>
+      </c>
+      <c r="I8" s="24">
+        <v>170</v>
+      </c>
+      <c r="J8" s="24">
+        <v>169</v>
+      </c>
+      <c r="K8" s="25"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="28" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="31">
+        <f>SUM(P8:U8) / div</f>
+        <v>-1.82</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8:P9" si="23">(E8-D8) * D$1</f>
+        <v>-30</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ref="Q8:Q9" si="24">(F8-E8) * E$1</f>
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ref="R8:R9" si="25">(G8-F8) * F$1</f>
+        <v>-35</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ref="S8:S9" si="26">(H8-G8) * G$1</f>
+        <v>-40</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8:T9" si="27">(I8-H8) * H$1</f>
+        <v>18</v>
+      </c>
+      <c r="U8">
+        <f t="shared" ref="U8:U9" si="28">(J8-I8) * I$1</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="23">
+        <f t="shared" si="6"/>
+        <v>176.85714285714286</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" si="7"/>
+        <v>7.0204081632653059</v>
+      </c>
+      <c r="D9" s="24">
+        <v>190</v>
+      </c>
+      <c r="E9" s="24">
+        <v>185</v>
+      </c>
+      <c r="F9" s="24">
+        <v>180</v>
+      </c>
+      <c r="G9" s="24">
+        <v>177</v>
+      </c>
+      <c r="H9" s="24">
+        <v>173</v>
+      </c>
+      <c r="I9" s="24">
+        <v>168</v>
+      </c>
+      <c r="J9" s="24">
+        <v>165</v>
+      </c>
+      <c r="K9" s="25"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="28" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="31">
+        <f>SUM(P9:U9) / div</f>
+        <v>-3.66</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="23"/>
+        <v>-25</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="24"/>
+        <v>-30</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="25"/>
+        <v>-21</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="26"/>
+        <v>-32</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="27"/>
+        <v>-45</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="28"/>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="23">
+        <f t="shared" si="6"/>
+        <v>179.4</v>
+      </c>
+      <c r="C10" s="23">
+        <f t="shared" si="7"/>
+        <v>6.7199999999999989</v>
+      </c>
+      <c r="D10" s="24">
+        <v>190</v>
+      </c>
+      <c r="E10" s="24">
+        <v>185</v>
+      </c>
+      <c r="F10" s="24">
+        <v>180</v>
+      </c>
+      <c r="G10" s="24">
+        <v>177</v>
+      </c>
+      <c r="H10" s="24">
+        <v>165</v>
+      </c>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="28" t="e">
+        <f t="shared" ref="N10" si="29">ABS(1 - (O10/L10))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" s="31">
+        <f>SUM(P10:U10) / div</f>
+        <v>-3.44</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10" si="30">(E10-D10) * D$1</f>
+        <v>-25</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10" si="31">(F10-E10) * E$1</f>
+        <v>-30</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ref="R10" si="32">(G10-F10) * F$1</f>
+        <v>-21</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ref="S10" si="33">(H10-G10) * G$1</f>
+        <v>-96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="23">
+        <f t="shared" si="6"/>
+        <v>179.4</v>
+      </c>
+      <c r="C11" s="23">
+        <f t="shared" si="7"/>
+        <v>6.7199999999999989</v>
+      </c>
+      <c r="D11" s="24">
+        <v>190</v>
+      </c>
+      <c r="E11" s="24">
+        <v>185</v>
+      </c>
+      <c r="F11" s="24">
+        <v>180</v>
+      </c>
+      <c r="G11" s="24">
+        <v>177</v>
+      </c>
+      <c r="H11" s="24">
+        <v>165</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="28" t="e">
+        <f t="shared" ref="N11" si="34">ABS(1 - (O11/L11))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" s="31">
+        <f>SUM(P11:U11) / div</f>
+        <v>-3.44</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11" si="35">(E11-D11) * D$1</f>
+        <v>-25</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ref="Q11" si="36">(F11-E11) * E$1</f>
+        <v>-30</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ref="R11" si="37">(G11-F11) * F$1</f>
+        <v>-21</v>
+      </c>
+      <c r="S11">
+        <f t="shared" ref="S11" si="38">(H11-G11) * G$1</f>
+        <v>-96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="23">
+        <f>AVERAGE(D12:J12)</f>
+        <v>187.85714285714286</v>
+      </c>
+      <c r="C12" s="23">
+        <f>AVEDEV(D12:J12)</f>
+        <v>4.4081632653061229</v>
+      </c>
+      <c r="D12">
+        <f>B21</f>
+        <v>182</v>
+      </c>
+      <c r="E12">
+        <f>B22</f>
+        <v>186</v>
+      </c>
+      <c r="F12">
+        <f>B23</f>
+        <v>181</v>
+      </c>
+      <c r="G12">
+        <f>B24</f>
+        <v>188</v>
+      </c>
+      <c r="H12">
+        <f>B25</f>
+        <v>201</v>
+      </c>
+      <c r="I12">
+        <f>B26</f>
+        <v>187</v>
+      </c>
+      <c r="J12">
+        <f>B27</f>
+        <v>190</v>
+      </c>
+      <c r="K12" s="25"/>
+      <c r="L12" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="M12" s="25"/>
+      <c r="N12" s="28" t="e">
+        <f t="shared" ref="N12" si="39">ABS(1 - (O12/L12))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O12" s="31">
+        <f>SUM(P12:U12) / div</f>
+        <v>2.86</v>
+      </c>
+      <c r="P12">
+        <f>(E12-D12) * D$1</f>
+        <v>20</v>
+      </c>
+      <c r="Q12">
+        <f>(F12-E12) * E$1</f>
+        <v>-30</v>
+      </c>
+      <c r="R12">
+        <f>(G12-F12) * F$1</f>
+        <v>49</v>
+      </c>
+      <c r="S12">
+        <f t="shared" ref="S12" si="40">(H12-G12) * G$1</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N13" s="23" t="e">
+        <f>AVERAGE(N2:N9)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>182</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="24">
+        <v>190</v>
+      </c>
+      <c r="G21" t="str">
+        <f>"Insert into @tblPace values(" &amp; E21 &amp; ", "  &amp; F21 &amp; ")"</f>
+        <v>Insert into @tblPace values(1, 190)</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>186</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="24">
+        <v>185</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ref="G22:G27" si="41">"Insert into @tblPace values(" &amp; E22 &amp; ", "  &amp; F22 &amp; ")"</f>
+        <v>Insert into @tblPace values(2, 185)</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>181</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" s="24">
+        <v>180</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="41"/>
+        <v>Insert into @tblPace values(3, 180)</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>188</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" s="24">
+        <v>177</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="41"/>
+        <v>Insert into @tblPace values(4, 177)</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>201</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25" s="24">
+        <v>165</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="41"/>
+        <v>Insert into @tblPace values(5, 165)</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>187</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26" s="24"/>
+      <c r="G26" t="str">
+        <f t="shared" si="41"/>
+        <v>Insert into @tblPace values(6, )</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>190</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27" s="24"/>
+      <c r="G27" t="str">
+        <f t="shared" si="41"/>
+        <v>Insert into @tblPace values(7, )</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>